<commit_message>
added some multithreading so the UI would get stuck
</commit_message>
<xml_diff>
--- a/PEATA/data/exports/test.xlsx
+++ b/PEATA/data/exports/test.xlsx
@@ -436,228 +436,228 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>view_count</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>share_count</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>video_duration</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>hashtag_info_list</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>hashtag_names</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>video_description</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>video_label</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>comment_count</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>create_time</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>video_mention_list</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>music_id</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>region_code</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>username</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>voice_to_text</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>is_stem_verified</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>like_count</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>region_code</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>video_description</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>video_label</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>view_count</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>music_id</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>share_count</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>voice_to_text</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>comment_count</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>create_time</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>hashtag_info_list</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>is_stem_verified</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>username</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>video_duration</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>video_mention_list</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>4315721</v>
+      </c>
+      <c r="B2" t="n">
+        <v>12149</v>
+      </c>
+      <c r="C2" t="n">
+        <v>62</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>[{'hashtag_name': 'firewings', 'hashtag_description': '', 'hashtag_id': 3979591}, {'hashtag_id': 47867, 'hashtag_name': 'chickenwing', 'hashtag_description': ''}, {'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}, {'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>['chickenwings', 'chickenwing', 'familygamenight', 'familygames', 'firewings', 'xyzbca']</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>252181</v>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Grab the Fire Wings #chickenwings #firewings #chickenwing #familygames #familygamenight #xyzbca </t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>{'content': '', 'sink': False, 'type': 0, 'vote': False, 'warn': False}</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2776</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1737777985</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K2" t="n">
+        <v>7.463699433146961e+18</v>
+      </c>
+      <c r="L2" t="n">
+        <v>7.463699553334824e+18</v>
+      </c>
+      <c r="M2" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Grab the Fire Wings #chickenwings #firewings #chickenwing #familygames #familygamenight #xyzbca </t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>{'content': '', 'sink': False, 'type': 0, 'vote': False, 'warn': False}</t>
-        </is>
-      </c>
-      <c r="F2" t="n">
-        <v>4315553</v>
-      </c>
-      <c r="G2" t="n">
-        <v>7.463699553334824e+18</v>
-      </c>
-      <c r="H2" t="n">
-        <v>12149</v>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>izzyandmarysdad</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t xml:space="preserve">Grab the fire wings. Buffalo. I wasn't paying attention. Carrots. Ranch. I got this. Mango habanero, peanut butter. Peanut butter. Peanut butter. Yeah, I guess, yeah. Barbecue. Ooh. French fries. Um, garlic Parmesan. Mango habanero. You don't want it. I already took this. Mango habanero. What is this? Oh, you gotta put it back, I guess. Carrots. I know. You try. Try what? Try it with ranch. Dragon what do you think of it? I think I like the wings better.
 </t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>2776</v>
-      </c>
-      <c r="K2" t="n">
-        <v>1737777985</v>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>[{'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}, {'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_id': 3979591, 'hashtag_name': 'firewings', 'hashtag_description': ''}, {'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}]</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>7.463699433146961e+18</v>
-      </c>
-      <c r="N2" t="b">
+      <c r="P2" t="b">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>izzyandmarysdad</t>
-        </is>
-      </c>
-      <c r="P2" t="n">
-        <v>62</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="Q2" t="n">
+        <v>252183</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>1721264</v>
+      </c>
+      <c r="B3" t="n">
+        <v>12316</v>
+      </c>
+      <c r="C3" t="n">
+        <v>112</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>[{'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_description': '', 'hashtag_id': 3979591, 'hashtag_name': 'firewings'}, {'hashtag_id': 47867, 'hashtag_name': 'chickenwing', 'hashtag_description': ''}, {'hashtag_name': 'familygames', 'hashtag_description': '', 'hashtag_id': 2556710}, {'hashtag_name': 'FamilyGameNight', 'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}]</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>['popeyes', 'familygamenight', 'familygames', 'popeyeschicken', 'popeyeschickensandwich', 'xyzbca']</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>71051</v>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Run for Popeyes Chicken #popeyes #popeyeschickensandwich #popeyeschicken #familygamenight #familygames #xyzbca </t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{'sink': False, 'type': 0, 'vote': False, 'warn': False, 'content': ''}</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2987</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1736387350</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>7.457726855131745e+18</v>
+      </c>
+      <c r="L3" t="n">
+        <v>7.457726829525323e+18</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>US</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Run for Popeyes Chicken #popeyes #popeyeschickensandwich #popeyeschicken #familygamenight #familygames #xyzbca </t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>{'content': '', 'sink': False, 'type': 0, 'vote': False, 'warn': False}</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>1721164</v>
-      </c>
-      <c r="G3" t="n">
-        <v>7.457726829525323e+18</v>
-      </c>
-      <c r="H3" t="n">
-        <v>12316</v>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>izzyandmarysdad</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t xml:space="preserve">Run for Papa's Chicken. Uh, two biscuits, I guess. Buffalo sauce, bro. It's too spicy. What? It just doesn't taste good. Chicken wings. Wait, you said wings. Wings. Okay, wait, this is not a wing? No. Chicken breast. Is this it? That's a thigh. This? Yeah. Um, classic chicken sandwich. All the strips, the Biscuits, Ranch. You have to come back. Um, legs. What's a leg? This? Yeah. Wait, more than one? Yeah, go ahead. Um, chicken thigh. What's that? Wait, the fries and the rest of the chicken, bro. What, you don't like fries
 </t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>2987</v>
-      </c>
-      <c r="K3" t="n">
-        <v>1736387350</v>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>[{'hashtag_description': '', 'hashtag_id': 2556710, 'hashtag_name': 'familygames'}, {'hashtag_description': "Whether it's desktop, table top, or old school, what are you playing for #FamilyGameNight?", 'hashtag_id': 287421, 'hashtag_name': 'FamilyGameNight'}, {'hashtag_description': 'Asla bir sonraki hamleni bilmelerine izin verme! 👀', 'hashtag_id': 1652484531221509, 'hashtag_name': 'xyzbca'}, {'hashtag_description': '', 'hashtag_id': 45455, 'hashtag_name': 'chickenwings'}, {'hashtag_description': '', 'hashtag_id': 3979591, 'hashtag_name': 'firewings'}, {'hashtag_description': '', 'hashtag_id': 47867, 'hashtag_name': 'chickenwing'}]</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>7.457726855131745e+18</v>
-      </c>
-      <c r="N3" t="b">
+      <c r="P3" t="b">
         <v>0</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>izzyandmarysdad</t>
-        </is>
-      </c>
-      <c r="P3" t="n">
-        <v>112</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>[]</t>
-        </is>
+      <c r="Q3" t="n">
+        <v>71051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>